<commit_message>
fix：basalt low optimization delete
</commit_message>
<xml_diff>
--- a/Dataset/Result/CamCalibrReslt.xlsx
+++ b/Dataset/Result/CamCalibrReslt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20380"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CamCalibrCode\Dataset\Result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7B2C56-D8DF-4685-A2B9-9FD6C95E4151}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAF0D0C-D16A-46F6-96B0-98B41452768E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{700934C4-4D82-4970-813A-54C320AF1DF3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>bluefox_artemis_night</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -100,6 +100,30 @@
   </si>
   <si>
     <t>optimize low</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>matlab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>opencv</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1982,15 +2006,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>533399</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:colOff>657224</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2315,10 +2339,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{611C63E3-6C02-4803-8E8A-9D9D79A4F4B0}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2329,9 +2353,11 @@
     <col min="4" max="4" width="12.625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C1">
         <v>20211125</v>
       </c>
@@ -2341,8 +2367,14 @@
       <c r="H1" t="s">
         <v>18</v>
       </c>
+      <c r="K1">
+        <v>20211216</v>
+      </c>
+      <c r="O1">
+        <v>20211214</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>16</v>
       </c>
@@ -2367,8 +2399,32 @@
       <c r="I2" t="s">
         <v>17</v>
       </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -2393,8 +2449,32 @@
       <c r="I3" t="s">
         <v>15</v>
       </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2423,7 +2503,7 @@
         <v>485.41574499364901</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -2452,7 +2532,7 @@
         <v>497.29911423608098</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -2480,8 +2560,32 @@
       <c r="I6">
         <v>496.38503549727199</v>
       </c>
+      <c r="J6">
+        <v>976.55712532041298</v>
+      </c>
+      <c r="K6">
+        <v>977.98019880099605</v>
+      </c>
+      <c r="L6">
+        <v>673.82457306168806</v>
+      </c>
+      <c r="M6">
+        <v>496.58406832349499</v>
+      </c>
+      <c r="N6">
+        <v>977.30332833</v>
+      </c>
+      <c r="O6">
+        <v>978.96299238999995</v>
+      </c>
+      <c r="P6">
+        <v>668.61445031000005</v>
+      </c>
+      <c r="Q6">
+        <v>500.89350610000002</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -2510,7 +2614,7 @@
         <v>494.70216874440501</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -2539,7 +2643,7 @@
         <v>499.42554065241001</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -2568,7 +2672,7 @@
         <v>497.86749264729002</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -2597,7 +2701,7 @@
         <v>496.13021854791702</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -2626,7 +2730,7 @@
         <v>352.75104472421901</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -2655,7 +2759,7 @@
         <v>360.81228620365499</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -2684,7 +2788,7 @@
         <v>358.69707256016397</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -2713,7 +2817,7 @@
         <v>357.45698310968697</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
feat: add some model
</commit_message>
<xml_diff>
--- a/Dataset/Result/CamCalibrReslt.xlsx
+++ b/Dataset/Result/CamCalibrReslt.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CamCalibrCode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CamCalibrCode\Dataset\Result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CE2879-8BA5-4465-9C65-D11929FD966C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF34F2E-B200-4D36-8884-6BE585DE3608}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{09F59CA0-44DD-4B04-B6E8-C57DCB2DEB30}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="45">
   <si>
     <t>bluefox_artemis_degenerate</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -183,10 +183,6 @@
   </si>
   <si>
     <t>reprojection error y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>std</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -289,7 +285,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -606,65 +602,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89B3D889-EC1D-439D-8CEA-E8B9FCCACCAB}">
-  <dimension ref="A1:O60"/>
+  <dimension ref="A1:N72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="23.75" customWidth="1"/>
-    <col min="5" max="5" width="18.625" customWidth="1"/>
-    <col min="6" max="6" width="19.25" customWidth="1"/>
-    <col min="7" max="7" width="13.5" customWidth="1"/>
-    <col min="8" max="8" width="12.625" customWidth="1"/>
-    <col min="9" max="9" width="12.875" customWidth="1"/>
-    <col min="10" max="10" width="12.75" customWidth="1"/>
-    <col min="15" max="15" width="13.625" customWidth="1"/>
+    <col min="3" max="3" width="23.75" customWidth="1"/>
+    <col min="4" max="4" width="18.625" customWidth="1"/>
+    <col min="5" max="5" width="19.25" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="12.625" customWidth="1"/>
+    <col min="8" max="8" width="12.875" customWidth="1"/>
+    <col min="9" max="9" width="12.75" customWidth="1"/>
+    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
         <v>0</v>
       </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -672,7 +670,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -680,7 +678,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -688,18 +686,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5">
         <v>20211125</v>
       </c>
-      <c r="D5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -710,43 +705,40 @@
         <v>974.91807890999996</v>
       </c>
       <c r="D6">
-        <v>0.93115625000000002</v>
+        <v>974.36902391000001</v>
       </c>
       <c r="E6">
-        <v>974.36902391000001</v>
+        <v>974.89649841000005</v>
       </c>
       <c r="F6">
-        <v>974.89649841000005</v>
+        <v>1044.1630405999999</v>
       </c>
       <c r="G6">
-        <v>1044.1630405999999</v>
+        <v>974.63222963999999</v>
       </c>
       <c r="H6">
-        <v>974.63222963999999</v>
+        <v>975.05538113</v>
       </c>
       <c r="I6">
-        <v>975.05538113</v>
+        <v>976.25894830000004</v>
       </c>
       <c r="J6">
-        <v>976.25894830000004</v>
+        <v>1014.0155104</v>
       </c>
       <c r="K6">
-        <v>1014.0155104</v>
+        <v>979.03957415000002</v>
       </c>
       <c r="L6">
-        <v>979.03957415000002</v>
+        <v>991.72351961000004</v>
       </c>
       <c r="M6">
-        <v>991.72351961000004</v>
+        <v>984.19117434999998</v>
       </c>
       <c r="N6">
-        <v>984.19117434999998</v>
-      </c>
-      <c r="O6">
         <v>915.27705366999999</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>21</v>
       </c>
@@ -754,43 +746,40 @@
         <v>976.83056263000003</v>
       </c>
       <c r="D7">
-        <v>0.90126488000000005</v>
+        <v>974.77661579000005</v>
       </c>
       <c r="E7">
-        <v>974.77661579000005</v>
+        <v>975.69977652</v>
       </c>
       <c r="F7">
-        <v>975.69977652</v>
+        <v>1043.1441212499999</v>
       </c>
       <c r="G7">
-        <v>1043.1441212499999</v>
+        <v>975.38016598000002</v>
       </c>
       <c r="H7">
-        <v>975.38016598000002</v>
+        <v>975.79151550999995</v>
       </c>
       <c r="I7">
-        <v>975.79151550999995</v>
+        <v>978.15630088</v>
       </c>
       <c r="J7">
-        <v>978.15630088</v>
+        <v>1011.24633483</v>
       </c>
       <c r="K7">
-        <v>1011.24633483</v>
+        <v>975.71493415999998</v>
       </c>
       <c r="L7">
-        <v>975.71493415999998</v>
+        <v>988.57470626999998</v>
       </c>
       <c r="M7">
-        <v>988.57470626999998</v>
+        <v>981.73499262999997</v>
       </c>
       <c r="N7">
-        <v>981.73499262999997</v>
-      </c>
-      <c r="O7">
         <v>912.10603903000003</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>22</v>
       </c>
@@ -798,43 +787,40 @@
         <v>670.45771646000003</v>
       </c>
       <c r="D8">
-        <v>0.97855358999999997</v>
-      </c>
-      <c r="E8">
         <v>674.22837643000003</v>
       </c>
-      <c r="F8">
+      <c r="E8" s="3">
         <v>668.92232629</v>
       </c>
-      <c r="G8">
+      <c r="F8" s="3">
         <v>664.35336566000001</v>
       </c>
-      <c r="H8">
+      <c r="G8" s="3">
         <v>668.29266882000002</v>
       </c>
-      <c r="I8">
+      <c r="H8" s="3">
         <v>664.16063186999997</v>
       </c>
-      <c r="J8">
+      <c r="I8" s="3">
         <v>659.34772351000004</v>
       </c>
-      <c r="K8">
+      <c r="J8" s="3">
         <v>650.26655261999997</v>
       </c>
-      <c r="L8">
+      <c r="K8" s="3">
         <v>633.00665663999996</v>
       </c>
-      <c r="M8">
+      <c r="L8" s="3">
         <v>636.67544424000005</v>
       </c>
-      <c r="N8">
+      <c r="M8" s="3">
         <v>630.18815526000003</v>
       </c>
-      <c r="O8">
+      <c r="N8" s="3">
         <v>632.17476227999998</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>23</v>
       </c>
@@ -842,43 +828,40 @@
         <v>501.00225083999999</v>
       </c>
       <c r="D9">
-        <v>0.92390298999999998</v>
-      </c>
-      <c r="E9">
         <v>499.03293481999998</v>
       </c>
-      <c r="F9">
+      <c r="E9" s="3">
         <v>501.47165517000002</v>
       </c>
-      <c r="G9">
+      <c r="F9" s="3">
         <v>494.71854105</v>
       </c>
-      <c r="H9">
+      <c r="G9" s="3">
         <v>502.63041340000001</v>
       </c>
-      <c r="I9">
+      <c r="H9" s="3">
         <v>501.15090445999999</v>
       </c>
-      <c r="J9">
+      <c r="I9" s="3">
         <v>503.12192270999998</v>
       </c>
-      <c r="K9">
+      <c r="J9" s="3">
         <v>354.79936932999999</v>
       </c>
-      <c r="L9">
+      <c r="K9" s="3">
         <v>359.33618876999998</v>
       </c>
-      <c r="M9">
+      <c r="L9" s="3">
         <v>361.44613648000001</v>
       </c>
-      <c r="N9">
+      <c r="M9" s="3">
         <v>357.92285902999998</v>
       </c>
-      <c r="O9">
+      <c r="N9" s="3">
         <v>349.51992281000003</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -889,13 +872,40 @@
         <v>-0.11309316</v>
       </c>
       <c r="D10">
-        <v>1.4880799999999999E-3</v>
-      </c>
-      <c r="F10">
+        <v>-0.11509844</v>
+      </c>
+      <c r="E10" s="3">
         <v>-0.11581716</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F10" s="3">
+        <v>-0.30033195000000001</v>
+      </c>
+      <c r="G10" s="3">
+        <v>-0.10690687</v>
+      </c>
+      <c r="H10" s="3">
+        <v>-0.10614796</v>
+      </c>
+      <c r="I10" s="3">
+        <v>-0.10357209000000001</v>
+      </c>
+      <c r="J10" s="3">
+        <v>3.5440119999999999E-2</v>
+      </c>
+      <c r="K10" s="3">
+        <v>5.6225329999999997E-2</v>
+      </c>
+      <c r="L10" s="3">
+        <v>4.28481E-2</v>
+      </c>
+      <c r="M10" s="3">
+        <v>7.1671860000000004E-2</v>
+      </c>
+      <c r="N10" s="3">
+        <v>0.11381123999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>28</v>
       </c>
@@ -903,13 +913,40 @@
         <v>9.9852910000000003E-2</v>
       </c>
       <c r="D11">
-        <v>2.4374700000000002E-3</v>
-      </c>
-      <c r="F11">
+        <v>0.10174748</v>
+      </c>
+      <c r="E11" s="3">
         <v>0.111052</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F11" s="3">
+        <v>0.10929431000000001</v>
+      </c>
+      <c r="G11" s="3">
+        <v>9.2973050000000002E-2</v>
+      </c>
+      <c r="H11" s="3">
+        <v>8.7379719999999994E-2</v>
+      </c>
+      <c r="I11" s="3">
+        <v>8.591915E-2</v>
+      </c>
+      <c r="J11" s="3">
+        <v>-3.9653319999999999E-2</v>
+      </c>
+      <c r="K11" s="3">
+        <v>-0.15317069</v>
+      </c>
+      <c r="L11" s="3">
+        <v>-0.12674849999999999</v>
+      </c>
+      <c r="M11" s="3">
+        <v>-0.21730210999999999</v>
+      </c>
+      <c r="N11" s="3">
+        <v>-0.25200052000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>29</v>
       </c>
@@ -917,13 +954,40 @@
         <v>6.5138999999999996E-4</v>
       </c>
       <c r="D12">
-        <v>2.2617000000000001E-4</v>
-      </c>
-      <c r="F12">
+        <v>1.8887E-4</v>
+      </c>
+      <c r="E12" s="3">
         <v>1.3311E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F12" s="3">
+        <v>-7.9820000000000005E-5</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1.55985E-3</v>
+      </c>
+      <c r="H12" s="3">
+        <v>2.0072800000000002E-3</v>
+      </c>
+      <c r="I12" s="3">
+        <v>2.1566100000000002E-3</v>
+      </c>
+      <c r="J12" s="3">
+        <v>6.9561999999999998E-4</v>
+      </c>
+      <c r="K12" s="3">
+        <v>-7.9936999999999999E-4</v>
+      </c>
+      <c r="L12" s="3">
+        <v>5.2139000000000005E-4</v>
+      </c>
+      <c r="M12" s="3">
+        <v>-3.2164999999999998E-4</v>
+      </c>
+      <c r="N12" s="3">
+        <v>-6.0300999999999996E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>30</v>
       </c>
@@ -931,13 +995,40 @@
         <v>-1.14135E-3</v>
       </c>
       <c r="D13">
-        <v>2.6212000000000002E-4</v>
-      </c>
-      <c r="F13">
+        <v>-3.2709999999999998E-4</v>
+      </c>
+      <c r="E13" s="3">
         <v>-1.5702699999999999E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F13" s="3">
+        <v>2.0378E-4</v>
+      </c>
+      <c r="G13" s="3">
+        <v>-1.8445200000000001E-3</v>
+      </c>
+      <c r="H13" s="3">
+        <v>-2.3595000000000001E-3</v>
+      </c>
+      <c r="I13" s="3">
+        <v>-3.90976E-3</v>
+      </c>
+      <c r="J13" s="3">
+        <v>1.5787900000000001E-3</v>
+      </c>
+      <c r="K13" s="3">
+        <v>2.73522E-3</v>
+      </c>
+      <c r="L13" s="3">
+        <v>1.37301E-3</v>
+      </c>
+      <c r="M13" s="3">
+        <v>7.0368000000000004E-4</v>
+      </c>
+      <c r="N13" s="3">
+        <v>3.9906000000000002E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -945,13 +1036,40 @@
         <v>3.9999999999999998E-6</v>
       </c>
       <c r="D14">
-        <v>0.167689</v>
-      </c>
-      <c r="F14">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="E14" s="3">
         <v>-1.9999999999999999E-6</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F14" s="3">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="G14" s="3">
+        <v>3.0000000000000001E-6</v>
+      </c>
+      <c r="H14" s="3">
+        <v>6.9999999999999999E-6</v>
+      </c>
+      <c r="I14" s="3">
+        <v>-1.5999999999999999E-5</v>
+      </c>
+      <c r="J14" s="3">
+        <v>-6.9999999999999999E-6</v>
+      </c>
+      <c r="K14" s="3">
+        <v>0</v>
+      </c>
+      <c r="L14" s="3">
+        <v>0</v>
+      </c>
+      <c r="M14" s="3">
+        <v>0</v>
+      </c>
+      <c r="N14" s="3">
+        <v>-1.9999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -959,21 +1077,70 @@
         <v>6.0000000000000002E-6</v>
       </c>
       <c r="D15">
-        <v>0.175922</v>
-      </c>
-      <c r="F15">
+        <v>-9.0000000000000002E-6</v>
+      </c>
+      <c r="E15" s="3">
         <v>1.9999999999999999E-6</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F15" s="3">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="G15" s="3">
+        <v>-3.9999999999999998E-6</v>
+      </c>
+      <c r="H15" s="3">
+        <v>6.0000000000000002E-6</v>
+      </c>
+      <c r="I15" s="3">
+        <v>-9.9999999999999995E-7</v>
+      </c>
+      <c r="J15" s="3">
+        <v>6.9999999999999999E-6</v>
+      </c>
+      <c r="K15" s="3">
+        <v>0</v>
+      </c>
+      <c r="L15" s="3">
+        <v>-9.9999999999999995E-7</v>
+      </c>
+      <c r="M15" s="3">
+        <v>-9.9999999999999995E-7</v>
+      </c>
+      <c r="N15" s="3">
+        <v>-6.0000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -984,8 +1151,16 @@
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -993,8 +1168,16 @@
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1005,8 +1188,16 @@
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1016,26 +1207,82 @@
       <c r="C21" s="3">
         <v>1072.3499999999999</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="D21" s="3">
+        <v>1076.6600000000001</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1098.8399999999999</v>
+      </c>
       <c r="F21" s="3">
-        <v>1098.8399999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+        <v>801.12900000000002</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1081.24</v>
+      </c>
+      <c r="H21" s="3">
+        <v>1081.24</v>
+      </c>
+      <c r="I21" s="3">
+        <v>1081.24</v>
+      </c>
+      <c r="J21" s="3">
+        <v>1007.52</v>
+      </c>
+      <c r="K21" s="3">
+        <v>999.19399999999996</v>
+      </c>
+      <c r="L21" s="3">
+        <v>1007.77</v>
+      </c>
+      <c r="M21" s="3">
+        <v>1009.12</v>
+      </c>
+      <c r="N21" s="3">
+        <v>925.29200000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="3">
         <v>1074.28</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="D22" s="3">
+        <v>1077.78</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1100.52</v>
+      </c>
       <c r="F22" s="3">
-        <v>1100.52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>800.79100000000005</v>
+      </c>
+      <c r="G22" s="3">
+        <v>1081.96</v>
+      </c>
+      <c r="H22" s="3">
+        <v>1081.96</v>
+      </c>
+      <c r="I22" s="3">
+        <v>1081.96</v>
+      </c>
+      <c r="J22" s="3">
+        <v>1005.31</v>
+      </c>
+      <c r="K22" s="3">
+        <v>998.20399999999995</v>
+      </c>
+      <c r="L22" s="3">
+        <v>1005.53</v>
+      </c>
+      <c r="M22" s="3">
+        <v>1007.09</v>
+      </c>
+      <c r="N22" s="3">
+        <v>921.13800000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23"/>
       <c r="B23" t="s">
         <v>22</v>
@@ -1043,13 +1290,41 @@
       <c r="C23" s="3">
         <v>673.98099999999999</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="D23" s="3">
+        <v>677.51700000000005</v>
+      </c>
+      <c r="E23" s="3">
+        <v>672.92</v>
+      </c>
       <c r="F23" s="3">
-        <v>672.92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>665.12900000000002</v>
+      </c>
+      <c r="G23" s="3">
+        <v>673.65700000000004</v>
+      </c>
+      <c r="H23" s="3">
+        <v>673.65700000000004</v>
+      </c>
+      <c r="I23" s="3">
+        <v>673.65700000000004</v>
+      </c>
+      <c r="J23" s="3">
+        <v>647.15099999999995</v>
+      </c>
+      <c r="K23" s="3">
+        <v>632.404</v>
+      </c>
+      <c r="L23" s="3">
+        <v>632.47699999999998</v>
+      </c>
+      <c r="M23" s="3">
+        <v>632.80899999999997</v>
+      </c>
+      <c r="N23" s="3">
+        <v>631.66300000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24"/>
       <c r="B24" t="s">
         <v>23</v>
@@ -1057,13 +1332,41 @@
       <c r="C24" s="3">
         <v>495.84399999999999</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="D24" s="3">
+        <v>497.286</v>
+      </c>
+      <c r="E24" s="3">
+        <v>496.39</v>
+      </c>
       <c r="F24" s="3">
-        <v>496.39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>494.69299999999998</v>
+      </c>
+      <c r="G24" s="3">
+        <v>499.42500000000001</v>
+      </c>
+      <c r="H24" s="3">
+        <v>499.42500000000001</v>
+      </c>
+      <c r="I24" s="3">
+        <v>499.42500000000001</v>
+      </c>
+      <c r="J24" s="3">
+        <v>352.74400000000003</v>
+      </c>
+      <c r="K24" s="3">
+        <v>360.85</v>
+      </c>
+      <c r="L24" s="3">
+        <v>358.60599999999999</v>
+      </c>
+      <c r="M24" s="3">
+        <v>357.529</v>
+      </c>
+      <c r="N24" s="3">
+        <v>353.46800000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25"/>
       <c r="B25" t="s">
         <v>34</v>
@@ -1071,13 +1374,41 @@
       <c r="C25" s="3">
         <v>0.106269</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="D25" s="3">
+        <v>9.8456299999999997E-2</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0.12606800000000001</v>
+      </c>
       <c r="F25" s="3">
-        <v>0.12606800000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>-0.23340900000000001</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0.110331</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0.110331</v>
+      </c>
+      <c r="I25" s="3">
+        <v>0.110331</v>
+      </c>
+      <c r="J25" s="3">
+        <v>-8.6332200000000005E-3</v>
+      </c>
+      <c r="K25" s="3">
+        <v>1.27169E-4</v>
+      </c>
+      <c r="L25" s="3">
+        <v>9.9390699999999995E-3</v>
+      </c>
+      <c r="M25" s="3">
+        <v>4.75101E-3</v>
+      </c>
+      <c r="N25" s="3">
+        <v>1.3766099999999999E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26"/>
       <c r="B26" t="s">
         <v>35</v>
@@ -1085,13 +1416,41 @@
       <c r="C26" s="3">
         <v>5.8031100000000002E-2</v>
       </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="D26" s="3">
+        <v>5.3404899999999998E-2</v>
+      </c>
+      <c r="E26" s="3">
+        <v>7.0171399999999995E-2</v>
+      </c>
       <c r="F26" s="3">
-        <v>7.0171399999999995E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0.55045900000000003</v>
+      </c>
+      <c r="G26" s="3">
+        <v>6.05126E-2</v>
+      </c>
+      <c r="H26" s="3">
+        <v>6.0512499999999997E-2</v>
+      </c>
+      <c r="I26" s="3">
+        <v>6.0512700000000003E-2</v>
+      </c>
+      <c r="J26" s="3">
+        <v>0</v>
+      </c>
+      <c r="K26" s="3">
+        <v>0</v>
+      </c>
+      <c r="L26" s="3">
+        <v>0</v>
+      </c>
+      <c r="M26" s="3">
+        <v>0</v>
+      </c>
+      <c r="N26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -1099,13 +1458,41 @@
       <c r="C27" s="3">
         <v>0.42056500000000002</v>
       </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+      <c r="D27" s="3">
+        <v>0.32139899999999999</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0.15276000000000001</v>
+      </c>
       <c r="F27" s="3">
-        <v>0.15276000000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>6.4026799999999995E-2</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0.63475300000000001</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0.63475300000000001</v>
+      </c>
+      <c r="I27" s="3">
+        <v>0.63475300000000001</v>
+      </c>
+      <c r="J27" s="3">
+        <v>0.400698</v>
+      </c>
+      <c r="K27" s="3">
+        <v>0.35143000000000002</v>
+      </c>
+      <c r="L27" s="3">
+        <v>0.47082499999999999</v>
+      </c>
+      <c r="M27" s="3">
+        <v>0.468468</v>
+      </c>
+      <c r="N27" s="3">
+        <v>0.63031599999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1113,13 +1500,41 @@
       <c r="C28" s="3">
         <v>6236.73</v>
       </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
+      <c r="D28" s="3">
+        <v>5247.06</v>
+      </c>
+      <c r="E28" s="3">
+        <v>3412.27</v>
+      </c>
       <c r="F28" s="3">
-        <v>3412.27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>1679.46</v>
+      </c>
+      <c r="G28" s="3">
+        <v>7434.43</v>
+      </c>
+      <c r="H28" s="3">
+        <v>7434.43</v>
+      </c>
+      <c r="I28" s="3">
+        <v>7434.43</v>
+      </c>
+      <c r="J28" s="3">
+        <v>20272.7</v>
+      </c>
+      <c r="K28" s="3">
+        <v>7209.59</v>
+      </c>
+      <c r="L28" s="3">
+        <v>8239.66</v>
+      </c>
+      <c r="M28" s="3">
+        <v>8244.32</v>
+      </c>
+      <c r="N28" s="3">
+        <v>28371.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -1127,246 +1542,579 @@
       <c r="C29" s="3">
         <v>0.45603500000000002</v>
       </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
+      <c r="D29" s="3">
+        <v>0.42994599999999999</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0.243316</v>
+      </c>
       <c r="F29" s="3">
-        <v>0.243316</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.202735</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0.55315700000000001</v>
+      </c>
+      <c r="H29" s="3">
+        <v>0.55315700000000001</v>
+      </c>
+      <c r="I29" s="3">
+        <v>0.55315700000000001</v>
+      </c>
+      <c r="J29" s="3">
+        <v>0.48104599999999997</v>
+      </c>
+      <c r="K29" s="3">
+        <v>0.49570900000000001</v>
+      </c>
+      <c r="L29" s="3">
+        <v>0.566689</v>
+      </c>
+      <c r="M29" s="3">
+        <v>0.57331900000000002</v>
+      </c>
+      <c r="N29" s="3">
+        <v>0.65867600000000004</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30"/>
+      <c r="B30"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+    </row>
+    <row r="31" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>13</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+    </row>
+    <row r="32" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>14</v>
+      </c>
+      <c r="B32" t="s">
+        <v>17</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+    </row>
+    <row r="33" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>15</v>
       </c>
+      <c r="B33"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+    </row>
+    <row r="34" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>16</v>
       </c>
-      <c r="B34">
-        <v>20211216</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B34"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+    </row>
+    <row r="35" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>26</v>
       </c>
       <c r="B35" t="s">
         <v>20</v>
       </c>
-      <c r="F35" s="4">
-        <v>976.55712532041298</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D35" s="3"/>
+      <c r="E35" s="3">
+        <v>991.33699999999999</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+    </row>
+    <row r="36" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36"/>
       <c r="B36" t="s">
         <v>21</v>
       </c>
-      <c r="F36" s="4">
-        <v>977.98019880099605</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D36" s="3"/>
+      <c r="E36" s="3">
+        <v>994.16700000000003</v>
+      </c>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+    </row>
+    <row r="37" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37"/>
       <c r="B37" t="s">
         <v>22</v>
       </c>
-      <c r="F37">
-        <v>673.82457306168806</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D37" s="3"/>
+      <c r="E37" s="3">
+        <v>673.11900000000003</v>
+      </c>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+    </row>
+    <row r="38" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38"/>
       <c r="B38" t="s">
         <v>23</v>
       </c>
-      <c r="F38">
+      <c r="D38" s="3"/>
+      <c r="E38" s="3">
+        <v>487.52199999999999</v>
+      </c>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+    </row>
+    <row r="39" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3">
+        <v>0.91605999999999999</v>
+      </c>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+    </row>
+    <row r="40" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3">
+        <v>9768.9699999999993</v>
+      </c>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+    </row>
+    <row r="41" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>37</v>
+      </c>
+      <c r="B41"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3">
+        <v>0.69658900000000001</v>
+      </c>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="3"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46">
+        <v>20211216</v>
+      </c>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="3"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" t="s">
+        <v>20</v>
+      </c>
+      <c r="E47" s="4">
+        <v>976.55712532041298</v>
+      </c>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>21</v>
+      </c>
+      <c r="E48" s="4">
+        <v>977.98019880099605</v>
+      </c>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="3"/>
+      <c r="N48" s="3"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>22</v>
+      </c>
+      <c r="E49" s="3">
+        <v>673.82457306168806</v>
+      </c>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="3"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>23</v>
+      </c>
+      <c r="E50" s="3">
         <v>496.58406832349499</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3"/>
+      <c r="L50" s="3"/>
+      <c r="M50" s="3"/>
+      <c r="N50" s="3"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>40</v>
+      </c>
+      <c r="B51" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51">
+        <v>-0.110160221624095</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>28</v>
+      </c>
+      <c r="E52">
+        <v>9.8677774133218904E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>41</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B53" t="s">
+        <v>29</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>30</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>42</v>
+      </c>
+      <c r="E55">
+        <v>0.23002407246565101</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>16</v>
+      </c>
+      <c r="B62">
+        <v>20211214</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>26</v>
+      </c>
+      <c r="B63" t="s">
+        <v>20</v>
+      </c>
+      <c r="E63">
+        <v>977.30332833</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
+        <v>21</v>
+      </c>
+      <c r="E64">
+        <v>978.96299238999995</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>22</v>
+      </c>
+      <c r="E65">
+        <v>668.61445031000005</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
+        <v>23</v>
+      </c>
+      <c r="E66">
+        <v>500.89350610000002</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>19</v>
+      </c>
+      <c r="B67" t="s">
         <v>27</v>
       </c>
-      <c r="F39">
-        <v>-0.110160221624095</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
+      <c r="E67">
+        <v>-0.11461281</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
         <v>28</v>
       </c>
-      <c r="F40">
-        <v>9.8677774133218904E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>42</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="E68">
+        <v>0.12946814000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
         <v>29</v>
       </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
+      <c r="E69">
+        <v>1.4266700000000001E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B70" t="s">
         <v>30</v>
       </c>
-      <c r="F42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="E70">
+        <v>-1.48431E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B71" t="s">
         <v>43</v>
       </c>
-      <c r="F43">
-        <v>0.23002407246565101</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>13</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>16</v>
-      </c>
-      <c r="B50">
-        <v>20211214</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>26</v>
-      </c>
-      <c r="B51" t="s">
-        <v>20</v>
-      </c>
-      <c r="F51">
-        <v>977.30332833</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B52" t="s">
-        <v>21</v>
-      </c>
-      <c r="F52">
-        <v>978.96299238999995</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
-        <v>22</v>
-      </c>
-      <c r="F53">
-        <v>668.61445031000005</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B54" t="s">
-        <v>23</v>
-      </c>
-      <c r="F54">
-        <v>500.89350610000002</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>19</v>
-      </c>
-      <c r="B55" t="s">
-        <v>27</v>
-      </c>
-      <c r="F55">
-        <v>-0.11461281</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B56" t="s">
-        <v>28</v>
-      </c>
-      <c r="F56">
-        <v>0.12946814000000001</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B57" t="s">
-        <v>29</v>
-      </c>
-      <c r="F57">
-        <v>1.4266700000000001E-3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B58" t="s">
-        <v>30</v>
-      </c>
-      <c r="F58">
-        <v>-1.48431E-3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B59" t="s">
+      <c r="E71">
+        <v>-4.6177059999999999E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>44</v>
       </c>
-      <c r="F59">
-        <v>-4.6177059999999999E-2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>45</v>
-      </c>
-      <c r="F60">
+      <c r="E72">
         <v>0.34789329373986699</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: 202206 some tests
</commit_message>
<xml_diff>
--- a/Dataset/Result/CamCalibrReslt.xlsx
+++ b/Dataset/Result/CamCalibrReslt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CamCalibrCode\Dataset\Result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52ABBCB-F5E3-4510-B497-6294DDD56323}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D0DEF9-3862-4117-9FE4-E47BAB4E66CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{09F59CA0-44DD-4B04-B6E8-C57DCB2DEB30}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="67">
   <si>
     <t>bluefox_artemis_degenerate</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -279,13 +279,25 @@
   </si>
   <si>
     <t>equidistant</t>
+  </si>
+  <si>
+    <t>intr_gs_40_5_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pinhole</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kalibr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,6 +330,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -347,7 +367,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -364,6 +384,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -680,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89B3D889-EC1D-439D-8CEA-E8B9FCCACCAB}">
-  <dimension ref="A1:W107"/>
+  <dimension ref="A1:X107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:U2"/>
+    <sheetView tabSelected="1" topLeftCell="H79" workbookViewId="0">
+      <selection activeCell="W110" sqref="W110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -703,9 +726,10 @@
     <col min="16" max="18" width="10.5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.75" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C1">
         <v>1</v>
       </c>
@@ -763,18 +787,21 @@
       <c r="U1">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G2" t="s">
@@ -822,40 +849,55 @@
       <c r="U2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6">
         <v>20211125</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W6">
+        <v>20220531</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -919,8 +961,11 @@
       <c r="U7">
         <v>809.70130953</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W7">
+        <v>741.13860871852103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>21</v>
       </c>
@@ -978,8 +1023,11 @@
       <c r="U8">
         <v>814.72442828999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W8">
+        <v>740.10935701444896</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>22</v>
       </c>
@@ -1037,8 +1085,11 @@
       <c r="U9">
         <v>496.15995865000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W9">
+        <v>641.52384619719101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>23</v>
       </c>
@@ -1096,8 +1147,11 @@
       <c r="U10">
         <v>369.66282631000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W10">
+        <v>513.47937451590406</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1158,8 +1212,11 @@
       <c r="U11">
         <v>5.1368619999999997E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W11">
+        <v>1.7812318374700299E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>28</v>
       </c>
@@ -1217,8 +1274,11 @@
       <c r="U12">
         <v>-0.12802358999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W12">
+        <v>1.9926210804139398E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>29</v>
       </c>
@@ -1276,8 +1336,11 @@
       <c r="U13">
         <v>2.0829999999999999E-4</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W13">
+        <v>1.4825144328253601E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>30</v>
       </c>
@@ -1335,8 +1398,11 @@
       <c r="U14">
         <v>-1.10614E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W14" s="5">
+        <v>-9.1220831206461405E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1394,8 +1460,11 @@
       <c r="U15">
         <v>5.0000000000000002E-5</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1452,6 +1521,9 @@
       </c>
       <c r="U16">
         <v>2.12E-4</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
@@ -1505,6 +1577,9 @@
       <c r="N17">
         <f t="shared" si="0"/>
         <v>6.3245553203367592E-6</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
@@ -2550,7 +2625,7 @@
       <c r="V48" s="3"/>
       <c r="W48" s="3"/>
     </row>
-    <row r="49" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49"/>
       <c r="B49"/>
       <c r="C49" s="3"/>
@@ -2579,7 +2654,7 @@
       <c r="V49" s="3"/>
       <c r="W49" s="3"/>
     </row>
-    <row r="50" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>13</v>
       </c>
@@ -2608,7 +2683,7 @@
       <c r="V50" s="3"/>
       <c r="W50" s="3"/>
     </row>
-    <row r="51" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>14</v>
       </c>
@@ -2637,7 +2712,7 @@
       <c r="V51" s="3"/>
       <c r="W51" s="3"/>
     </row>
-    <row r="52" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>15</v>
       </c>
@@ -2664,7 +2739,7 @@
       <c r="V52" s="3"/>
       <c r="W52" s="3"/>
     </row>
-    <row r="53" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>16</v>
       </c>
@@ -2691,7 +2766,7 @@
       <c r="V53" s="3"/>
       <c r="W53" s="3"/>
     </row>
-    <row r="54" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>26</v>
       </c>
@@ -2719,7 +2794,7 @@
       <c r="U54" s="3"/>
       <c r="V54" s="3"/>
     </row>
-    <row r="55" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55"/>
       <c r="B55" t="s">
         <v>21</v>
@@ -2745,7 +2820,7 @@
       <c r="U55" s="3"/>
       <c r="V55" s="3"/>
     </row>
-    <row r="56" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56"/>
       <c r="B56" t="s">
         <v>22</v>
@@ -2771,7 +2846,7 @@
       <c r="U56" s="3"/>
       <c r="V56" s="3"/>
     </row>
-    <row r="57" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57"/>
       <c r="B57" t="s">
         <v>23</v>
@@ -2789,7 +2864,7 @@
       <c r="M57" s="3"/>
       <c r="N57" s="3"/>
     </row>
-    <row r="58" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>36</v>
       </c>
@@ -2808,7 +2883,7 @@
       <c r="M58" s="3"/>
       <c r="N58" s="3"/>
     </row>
-    <row r="59" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>31</v>
       </c>
@@ -2827,7 +2902,7 @@
       <c r="M59" s="3"/>
       <c r="N59" s="3"/>
     </row>
-    <row r="60" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>37</v>
       </c>
@@ -2845,8 +2920,16 @@
       <c r="L60" s="3"/>
       <c r="M60" s="3"/>
       <c r="N60" s="3"/>
-    </row>
-    <row r="61" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q60" s="3"/>
+      <c r="R60" s="3"/>
+      <c r="S60" s="3"/>
+      <c r="T60" s="3"/>
+      <c r="U60" s="3"/>
+      <c r="V60" s="3"/>
+      <c r="W60" s="3"/>
+      <c r="X60" s="3"/>
+    </row>
+    <row r="61" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61"/>
       <c r="B61"/>
       <c r="D61" s="3"/>
@@ -2860,8 +2943,16 @@
       <c r="L61" s="3"/>
       <c r="M61" s="3"/>
       <c r="N61" s="3"/>
-    </row>
-    <row r="62" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q61" s="3"/>
+      <c r="R61" s="3"/>
+      <c r="S61" s="3"/>
+      <c r="T61" s="3"/>
+      <c r="U61" s="3"/>
+      <c r="V61" s="3"/>
+      <c r="W61" s="3"/>
+      <c r="X61" s="3"/>
+    </row>
+    <row r="62" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>13</v>
       </c>
@@ -2879,8 +2970,16 @@
       <c r="L62" s="3"/>
       <c r="M62" s="3"/>
       <c r="N62" s="3"/>
-    </row>
-    <row r="63" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q62" s="3"/>
+      <c r="R62" s="3"/>
+      <c r="S62" s="3"/>
+      <c r="T62" s="3"/>
+      <c r="U62" s="3"/>
+      <c r="V62" s="3"/>
+      <c r="W62" s="3"/>
+      <c r="X62" s="3"/>
+    </row>
+    <row r="63" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -2898,8 +2997,16 @@
       <c r="L63" s="3"/>
       <c r="M63" s="3"/>
       <c r="N63" s="3"/>
-    </row>
-    <row r="64" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q63" s="3"/>
+      <c r="R63" s="3"/>
+      <c r="S63" s="3"/>
+      <c r="T63" s="3"/>
+      <c r="U63" s="3"/>
+      <c r="V63" s="3"/>
+      <c r="W63" s="3"/>
+      <c r="X63" s="3"/>
+    </row>
+    <row r="64" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>15</v>
       </c>
@@ -2915,8 +3022,16 @@
       <c r="L64" s="3"/>
       <c r="M64" s="3"/>
       <c r="N64" s="3"/>
-    </row>
-    <row r="65" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q64" s="3"/>
+      <c r="R64" s="3"/>
+      <c r="S64" s="3"/>
+      <c r="T64" s="3"/>
+      <c r="U64" s="3"/>
+      <c r="V64" s="3"/>
+      <c r="W64" s="3"/>
+      <c r="X64" s="3"/>
+    </row>
+    <row r="65" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>16</v>
       </c>
@@ -2932,8 +3047,16 @@
       <c r="L65" s="3"/>
       <c r="M65" s="3"/>
       <c r="N65" s="3"/>
-    </row>
-    <row r="66" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q65" s="3"/>
+      <c r="R65" s="3"/>
+      <c r="S65" s="3"/>
+      <c r="T65" s="3"/>
+      <c r="U65" s="3"/>
+      <c r="V65" s="3"/>
+      <c r="W65" s="3"/>
+      <c r="X65" s="3"/>
+    </row>
+    <row r="66" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>26</v>
       </c>
@@ -2953,8 +3076,18 @@
       <c r="L66" s="3"/>
       <c r="M66" s="3"/>
       <c r="N66" s="3"/>
-    </row>
-    <row r="67" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q66" s="3"/>
+      <c r="R66" s="3"/>
+      <c r="S66" s="3"/>
+      <c r="T66" s="3"/>
+      <c r="U66" s="3"/>
+      <c r="V66" s="3"/>
+      <c r="W66" s="3">
+        <v>741.32413181142203</v>
+      </c>
+      <c r="X66" s="3"/>
+    </row>
+    <row r="67" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67"/>
       <c r="B67" t="s">
         <v>21</v>
@@ -2972,8 +3105,18 @@
       <c r="L67" s="3"/>
       <c r="M67" s="3"/>
       <c r="N67" s="3"/>
-    </row>
-    <row r="68" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q67" s="3"/>
+      <c r="R67" s="3"/>
+      <c r="S67" s="3"/>
+      <c r="T67" s="3"/>
+      <c r="U67" s="3"/>
+      <c r="V67" s="3"/>
+      <c r="W67" s="3">
+        <v>740.39603121738799</v>
+      </c>
+      <c r="X67" s="3"/>
+    </row>
+    <row r="68" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68"/>
       <c r="B68" t="s">
         <v>22</v>
@@ -2991,8 +3134,18 @@
       <c r="L68" s="3"/>
       <c r="M68" s="3"/>
       <c r="N68" s="3"/>
-    </row>
-    <row r="69" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q68" s="3"/>
+      <c r="R68" s="3"/>
+      <c r="S68" s="3"/>
+      <c r="T68" s="3"/>
+      <c r="U68" s="3"/>
+      <c r="V68" s="3"/>
+      <c r="W68" s="3">
+        <v>641.41312692925896</v>
+      </c>
+      <c r="X68" s="3"/>
+    </row>
+    <row r="69" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69"/>
       <c r="B69" t="s">
         <v>23</v>
@@ -3010,8 +3163,18 @@
       <c r="L69" s="3"/>
       <c r="M69" s="3"/>
       <c r="N69" s="3"/>
-    </row>
-    <row r="70" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q69" s="3"/>
+      <c r="R69" s="3"/>
+      <c r="S69" s="3"/>
+      <c r="T69" s="3"/>
+      <c r="U69" s="3"/>
+      <c r="V69" s="3"/>
+      <c r="W69" s="3">
+        <v>513.26932070095302</v>
+      </c>
+      <c r="X69" s="3"/>
+    </row>
+    <row r="70" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70"/>
       <c r="B70" t="s">
         <v>59</v>
@@ -3029,8 +3192,18 @@
       <c r="L70" s="3"/>
       <c r="M70" s="3"/>
       <c r="N70" s="3"/>
-    </row>
-    <row r="71" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q70" s="3"/>
+      <c r="R70" s="3"/>
+      <c r="S70" s="3"/>
+      <c r="T70" s="3"/>
+      <c r="U70" s="3"/>
+      <c r="V70" s="3"/>
+      <c r="W70" s="3">
+        <v>1.8331507764619899E-2</v>
+      </c>
+      <c r="X70" s="3"/>
+    </row>
+    <row r="71" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71"/>
       <c r="B71" t="s">
         <v>60</v>
@@ -3048,8 +3221,18 @@
       <c r="L71" s="3"/>
       <c r="M71" s="3"/>
       <c r="N71" s="3"/>
-    </row>
-    <row r="72" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q71" s="3"/>
+      <c r="R71" s="3"/>
+      <c r="S71" s="3"/>
+      <c r="T71" s="3"/>
+      <c r="U71" s="3"/>
+      <c r="V71" s="3"/>
+      <c r="W71" s="3">
+        <v>6.7836828867549805E-4</v>
+      </c>
+      <c r="X71" s="3"/>
+    </row>
+    <row r="72" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72"/>
       <c r="B72" t="s">
         <v>61</v>
@@ -3067,8 +3250,18 @@
       <c r="L72" s="3"/>
       <c r="M72" s="3"/>
       <c r="N72" s="3"/>
-    </row>
-    <row r="73" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q72" s="3"/>
+      <c r="R72" s="3"/>
+      <c r="S72" s="3"/>
+      <c r="T72" s="3"/>
+      <c r="U72" s="3"/>
+      <c r="V72" s="3"/>
+      <c r="W72" s="3">
+        <v>3.5957972213757701E-3</v>
+      </c>
+      <c r="X72" s="3"/>
+    </row>
+    <row r="73" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73"/>
       <c r="B73" t="s">
         <v>62</v>
@@ -3086,8 +3279,18 @@
       <c r="L73" s="3"/>
       <c r="M73" s="3"/>
       <c r="N73" s="3"/>
-    </row>
-    <row r="74" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q73" s="3"/>
+      <c r="R73" s="3"/>
+      <c r="S73" s="3"/>
+      <c r="T73" s="3"/>
+      <c r="U73" s="3"/>
+      <c r="V73" s="3"/>
+      <c r="W73" s="3">
+        <v>-1.2919691421533501E-3</v>
+      </c>
+      <c r="X73" s="3"/>
+    </row>
+    <row r="74" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>36</v>
       </c>
@@ -3105,8 +3308,18 @@
       <c r="L74" s="3"/>
       <c r="M74" s="3"/>
       <c r="N74" s="3"/>
-    </row>
-    <row r="75" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q74" s="3"/>
+      <c r="R74" s="3"/>
+      <c r="S74" s="3"/>
+      <c r="T74" s="3"/>
+      <c r="U74" s="3"/>
+      <c r="V74" s="3"/>
+      <c r="W74" s="3">
+        <v>2.0262100000000002E-2</v>
+      </c>
+      <c r="X74" s="3"/>
+    </row>
+    <row r="75" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>31</v>
       </c>
@@ -3124,8 +3337,18 @@
       <c r="L75" s="3"/>
       <c r="M75" s="3"/>
       <c r="N75" s="3"/>
-    </row>
-    <row r="76" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q75" s="3"/>
+      <c r="R75" s="3"/>
+      <c r="S75" s="3"/>
+      <c r="T75" s="3"/>
+      <c r="U75" s="3"/>
+      <c r="V75" s="3"/>
+      <c r="W75" s="3">
+        <v>9638.17</v>
+      </c>
+      <c r="X75" s="3"/>
+    </row>
+    <row r="76" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>37</v>
       </c>
@@ -3143,8 +3366,16 @@
       <c r="L76" s="3"/>
       <c r="M76" s="3"/>
       <c r="N76" s="3"/>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S76" s="3"/>
+      <c r="T76" s="3"/>
+      <c r="U76" s="3"/>
+      <c r="V76" s="3"/>
+      <c r="W76" s="3">
+        <v>0.12055</v>
+      </c>
+      <c r="X76" s="3"/>
+    </row>
+    <row r="77" spans="1:24" x14ac:dyDescent="0.2">
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
@@ -3157,8 +3388,14 @@
       <c r="L77" s="3"/>
       <c r="M77" s="3"/>
       <c r="N77" s="3"/>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S77" s="3"/>
+      <c r="T77" s="3"/>
+      <c r="U77" s="3"/>
+      <c r="V77" s="3"/>
+      <c r="W77" s="3"/>
+      <c r="X77" s="3"/>
+    </row>
+    <row r="78" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>13</v>
       </c>
@@ -3177,8 +3414,14 @@
       <c r="L78" s="3"/>
       <c r="M78" s="3"/>
       <c r="N78" s="3"/>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S78" s="3"/>
+      <c r="T78" s="3"/>
+      <c r="U78" s="3"/>
+      <c r="V78" s="3"/>
+      <c r="W78" s="3"/>
+      <c r="X78" s="3"/>
+    </row>
+    <row r="79" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>14</v>
       </c>
@@ -3194,8 +3437,14 @@
       <c r="L79" s="3"/>
       <c r="M79" s="3"/>
       <c r="N79" s="3"/>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S79" s="3"/>
+      <c r="T79" s="3"/>
+      <c r="U79" s="3"/>
+      <c r="V79" s="3"/>
+      <c r="W79" s="3"/>
+      <c r="X79" s="3"/>
+    </row>
+    <row r="80" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>15</v>
       </c>
@@ -3211,8 +3460,14 @@
       <c r="L80" s="3"/>
       <c r="M80" s="3"/>
       <c r="N80" s="3"/>
-    </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="S80" s="3"/>
+      <c r="T80" s="3"/>
+      <c r="U80" s="3"/>
+      <c r="V80" s="3"/>
+      <c r="W80" s="3"/>
+      <c r="X80" s="3"/>
+    </row>
+    <row r="81" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>16</v>
       </c>
@@ -3229,8 +3484,14 @@
       <c r="L81" s="3"/>
       <c r="M81" s="3"/>
       <c r="N81" s="3"/>
-    </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="S81" s="3"/>
+      <c r="T81" s="3"/>
+      <c r="U81" s="3"/>
+      <c r="V81" s="3"/>
+      <c r="W81" s="3"/>
+      <c r="X81" s="3"/>
+    </row>
+    <row r="82" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>26</v>
       </c>
@@ -3254,11 +3515,16 @@
       <c r="P82" t="s">
         <v>48</v>
       </c>
-      <c r="U82" t="s">
+      <c r="S82" s="3"/>
+      <c r="T82" s="3"/>
+      <c r="U82" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V82" s="3"/>
+      <c r="W82" s="3"/>
+      <c r="X82" s="3"/>
+    </row>
+    <row r="83" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>21</v>
       </c>
@@ -3280,7 +3546,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>22</v>
       </c>
@@ -3299,7 +3565,7 @@
       <c r="M84" s="3"/>
       <c r="N84" s="3"/>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
         <v>23</v>
       </c>
@@ -3318,7 +3584,7 @@
       <c r="M85" s="3"/>
       <c r="N85" s="3"/>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>40</v>
       </c>
@@ -3332,7 +3598,7 @@
         <v>-0.29569018103178002</v>
       </c>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>28</v>
       </c>
@@ -3343,7 +3609,7 @@
         <v>0.10259711547492301</v>
       </c>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>41</v>
       </c>
@@ -3357,7 +3623,7 @@
         <v>-9.7278384628337697E-5</v>
       </c>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>30</v>
       </c>
@@ -3368,7 +3634,7 @@
         <v>2.2107402436058701E-4</v>
       </c>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>42</v>
       </c>
@@ -3385,7 +3651,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>13</v>
       </c>
@@ -3393,17 +3659,17 @@
         <v>25</v>
       </c>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>16</v>
       </c>
@@ -3411,7 +3677,7 @@
         <v>20211214</v>
       </c>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>26</v>
       </c>
@@ -3427,8 +3693,11 @@
       <c r="T98">
         <v>14839.73738348</v>
       </c>
-    </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W98">
+        <v>741.36777522</v>
+      </c>
+    </row>
+    <row r="99" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
         <v>21</v>
       </c>
@@ -3441,8 +3710,11 @@
       <c r="T99">
         <v>13894.696526719999</v>
       </c>
-    </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W99">
+        <v>740.22092375</v>
+      </c>
+    </row>
+    <row r="100" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
         <v>22</v>
       </c>
@@ -3455,8 +3727,11 @@
       <c r="T100">
         <v>639.96850023000002</v>
       </c>
-    </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W100">
+        <v>639.99067258000002</v>
+      </c>
+    </row>
+    <row r="101" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
         <v>23</v>
       </c>
@@ -3469,8 +3744,11 @@
       <c r="T101">
         <v>478.8815305</v>
       </c>
-    </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W101">
+        <v>515.48692446999996</v>
+      </c>
+    </row>
+    <row r="102" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>19</v>
       </c>
@@ -3486,8 +3764,11 @@
       <c r="T102">
         <v>3.6861551000000001</v>
       </c>
-    </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W102">
+        <v>-0.28463873000000001</v>
+      </c>
+    </row>
+    <row r="103" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
         <v>28</v>
       </c>
@@ -3500,8 +3781,11 @@
       <c r="T103">
         <v>865.38231173999998</v>
       </c>
-    </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W103">
+        <v>9.7633609999999996E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>29</v>
       </c>
@@ -3514,8 +3798,11 @@
       <c r="T104">
         <v>0.45370999000000001</v>
       </c>
-    </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W104">
+        <v>-1.7802000000000001E-4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
         <v>30</v>
       </c>
@@ -3528,8 +3815,11 @@
       <c r="T105">
         <v>4.1710009999999999E-2</v>
       </c>
-    </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W105">
+        <v>1.013E-5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
         <v>43</v>
       </c>
@@ -3542,8 +3832,11 @@
       <c r="T106">
         <v>1.1412876300000001</v>
       </c>
-    </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W106">
+        <v>-1.6098060000000001E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>44</v>
       </c>
@@ -3555,6 +3848,9 @@
       </c>
       <c r="T107">
         <v>0.38358855700799999</v>
+      </c>
+      <c r="W107">
+        <v>0.35199544170000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>